<commit_message>
[UPDATE] Se organiza la información relacionada al avance actual del proyecto [TFM]
</commit_message>
<xml_diff>
--- a/Proyecto_TFM/Models/HeadTailDetec/ComparacionResultados.xlsx
+++ b/Proyecto_TFM/Models/HeadTailDetec/ComparacionResultados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unirioja-my.sharepoint.com/personal/migomesu_unirioja_es/Documents/RepositoriosPersonales/TrabajosMaestriaCienciadeDatos/Proyecto_TFM/Models/HeadTailDetec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{C15D7F6A-1DA3-4EF6-8F01-37F6B3667E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6085D8F8-6CD3-4F08-A812-36BDF2313FED}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{C15D7F6A-1DA3-4EF6-8F01-37F6B3667E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09A88F10-D0D9-4F79-923F-6247D6B2CD77}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03E4A7EE-F405-4C82-91AB-758C70449BFF}"/>
+    <workbookView xWindow="-21564" yWindow="1008" windowWidth="21660" windowHeight="11328" xr2:uid="{03E4A7EE-F405-4C82-91AB-758C70449BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -94,12 +94,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -123,14 +129,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9199EF-6AD9-4985-8F47-CB3B5E524477}">
   <dimension ref="D8:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,10 +560,10 @@
       <c r="F12" s="3">
         <v>0.63187000000000004</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="5">
         <v>0.74494000000000005</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="5">
         <v>0.73602999999999996</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[UPDATE] Se incluye la distancia uclidea para las trayectorias de seguimiento. [Ajustes Finales TFM]
</commit_message>
<xml_diff>
--- a/Proyecto_TFM/Models/HeadTailDetec/ComparacionResultados.xlsx
+++ b/Proyecto_TFM/Models/HeadTailDetec/ComparacionResultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unirioja-my.sharepoint.com/personal/migomesu_unirioja_es/Documents/RepositoriosPersonales/TrabajosMaestriaCienciadeDatos/Proyecto_TFM/Models/HeadTailDetec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{C15D7F6A-1DA3-4EF6-8F01-37F6B3667E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09A88F10-D0D9-4F79-923F-6247D6B2CD77}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{C15D7F6A-1DA3-4EF6-8F01-37F6B3667E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FD6F470-541F-47CD-B5B4-2175C240F7AE}"/>
   <bookViews>
-    <workbookView xWindow="-21564" yWindow="1008" windowWidth="21660" windowHeight="11328" xr2:uid="{03E4A7EE-F405-4C82-91AB-758C70449BFF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{03E4A7EE-F405-4C82-91AB-758C70449BFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Tamaño Imagen Entrada</t>
   </si>
@@ -62,17 +62,27 @@
     <t>Tipo de Modelo (1000 Epochs)</t>
   </si>
   <si>
-    <t>Map 50</t>
+    <t>mAP 50</t>
+  </si>
+  <si>
+    <t>mAP 50 - 95</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +102,14 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -129,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -138,6 +156,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9199EF-6AD9-4985-8F47-CB3B5E524477}">
-  <dimension ref="D8:H13"/>
+  <dimension ref="D7:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +514,15 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
@@ -500,25 +538,31 @@
       <c r="H8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>640</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>0.78403999999999996</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="9">
         <v>0.67908999999999997</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="5">
         <v>0.74933000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="5">
+        <v>0.32995000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="3">
         <v>250</v>
@@ -532,8 +576,11 @@
       <c r="H10" s="3">
         <v>0.76917000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="3">
+        <v>0.31130999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
@@ -549,42 +596,182 @@
       <c r="H11" s="3">
         <v>0.71016000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="3">
+        <v>0.30060999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="12">
         <v>640</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="12">
         <v>0.63187000000000004</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="12">
         <v>0.74494000000000005</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="12">
         <v>0.73602999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="s">
+      <c r="I12" s="13">
+        <v>0.32163999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="7">
         <v>640</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="7">
         <v>0.73860999999999999</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="7">
         <v>0.71443000000000001</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="7">
         <v>0.72819</v>
       </c>
+      <c r="I13" s="8">
+        <v>0.31159999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3">
+        <v>640</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="G18">
+        <v>0.73</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="2"/>
+      <c r="E19" s="3">
+        <v>250</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="3">
+        <v>640</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.314</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="5">
+        <v>640</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.34499999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="7">
+        <v>640</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0.754</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.33</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F16:I16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>